<commit_message>
Fix pjm 5-bus case for UC
</commit_message>
<xml_diff>
--- a/ams/cases/5bus/pjm5bus_uced.xlsx
+++ b/ams/cases/5bus/pjm5bus_uced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/ams/ams/cases/5bus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4480CC0E-9266-E44D-853A-6C85F866F599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{844ECDA7-4567-8542-97E2-144FADC54E13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21600" yWindow="2660" windowWidth="21600" windowHeight="18940" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="21" r:id="rId1"/>
@@ -18,19 +18,18 @@
     <sheet name="PQ" sheetId="2" r:id="rId3"/>
     <sheet name="PV" sheetId="3" r:id="rId4"/>
     <sheet name="Slack" sheetId="4" r:id="rId5"/>
-    <sheet name="Line" sheetId="5" r:id="rId6"/>
-    <sheet name="Area" sheetId="6" r:id="rId7"/>
-    <sheet name="Region" sheetId="10" r:id="rId8"/>
-    <sheet name="GCost" sheetId="11" r:id="rId9"/>
+    <sheet name="GCost" sheetId="11" r:id="rId6"/>
+    <sheet name="Line" sheetId="5" r:id="rId7"/>
+    <sheet name="Area" sheetId="6" r:id="rId8"/>
+    <sheet name="Region" sheetId="10" r:id="rId9"/>
     <sheet name="EDTSlot" sheetId="12" r:id="rId10"/>
     <sheet name="UCTSlot" sheetId="13" r:id="rId11"/>
-    <sheet name="DCost" sheetId="14" r:id="rId12"/>
-    <sheet name="SFR" sheetId="15" r:id="rId13"/>
-    <sheet name="SFRCost" sheetId="16" r:id="rId14"/>
-    <sheet name="SR" sheetId="17" r:id="rId15"/>
-    <sheet name="SRCost" sheetId="18" r:id="rId16"/>
-    <sheet name="NSR" sheetId="19" r:id="rId17"/>
-    <sheet name="NSRCost" sheetId="20" r:id="rId18"/>
+    <sheet name="SFR" sheetId="15" r:id="rId12"/>
+    <sheet name="SFRCost" sheetId="16" r:id="rId13"/>
+    <sheet name="SR" sheetId="17" r:id="rId14"/>
+    <sheet name="SRCost" sheetId="18" r:id="rId15"/>
+    <sheet name="NSR" sheetId="19" r:id="rId16"/>
+    <sheet name="NSRCost" sheetId="20" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="218">
   <si>
     <t>idx</t>
   </si>
@@ -508,27 +507,12 @@
     <t>UCT24</t>
   </si>
   <si>
-    <t>load</t>
-  </si>
-  <si>
-    <t>cd</t>
-  </si>
-  <si>
-    <t>Dcost_1</t>
-  </si>
-  <si>
     <t>PQ_1</t>
   </si>
   <si>
-    <t>Dcost_2</t>
-  </si>
-  <si>
     <t>PQ_2</t>
   </si>
   <si>
-    <t>Dcost_3</t>
-  </si>
-  <si>
     <t>PQ_3</t>
   </si>
   <si>
@@ -698,6 +682,27 @@
   </si>
   <si>
     <t>td2</t>
+  </si>
+  <si>
+    <t>du</t>
+  </si>
+  <si>
+    <t>dd</t>
+  </si>
+  <si>
+    <t>SFR1</t>
+  </si>
+  <si>
+    <t>SFR2</t>
+  </si>
+  <si>
+    <t>rate_a</t>
+  </si>
+  <si>
+    <t>rate_b</t>
+  </si>
+  <si>
+    <t>rate_c</t>
   </si>
 </sst>
 </file>
@@ -809,7 +814,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -825,21 +830,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1159,16 +1158,16 @@
         <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1176,23 +1175,23 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>208</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+        <v>203</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C3" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1200,10 +1199,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C4" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -1246,7 +1245,7 @@
         <v>80</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1260,7 +1259,7 @@
         <v>82</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1274,7 +1273,7 @@
         <v>84</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1288,7 +1287,7 @@
         <v>86</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1302,7 +1301,7 @@
         <v>88</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1316,7 +1315,7 @@
         <v>90</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1330,7 +1329,7 @@
         <v>92</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1344,7 +1343,7 @@
         <v>94</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1358,7 +1357,7 @@
         <v>96</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1372,7 +1371,7 @@
         <v>98</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1386,7 +1385,7 @@
         <v>100</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1400,7 +1399,7 @@
         <v>102</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1414,7 +1413,7 @@
         <v>104</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1428,7 +1427,7 @@
         <v>106</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1442,7 +1441,7 @@
         <v>108</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1456,7 +1455,7 @@
         <v>110</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1498,7 +1497,7 @@
         <v>116</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1512,7 +1511,7 @@
         <v>119</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1526,7 +1525,7 @@
         <v>121</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1540,7 +1539,7 @@
         <v>123</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1554,7 +1553,7 @@
         <v>125</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1568,7 +1567,7 @@
         <v>127</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -1581,7 +1580,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1611,7 +1610,7 @@
         <v>128</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1625,7 +1624,7 @@
         <v>129</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1639,7 +1638,7 @@
         <v>130</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1653,7 +1652,7 @@
         <v>131</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1667,7 +1666,7 @@
         <v>132</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1681,7 +1680,7 @@
         <v>133</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1695,7 +1694,7 @@
         <v>134</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1709,7 +1708,7 @@
         <v>135</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1723,7 +1722,7 @@
         <v>136</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1737,7 +1736,7 @@
         <v>137</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1751,7 +1750,7 @@
         <v>138</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1765,7 +1764,7 @@
         <v>139</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1779,7 +1778,7 @@
         <v>140</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1793,7 +1792,7 @@
         <v>141</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1807,7 +1806,7 @@
         <v>142</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1821,7 +1820,7 @@
         <v>143</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1863,7 +1862,7 @@
         <v>146</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1877,7 +1876,7 @@
         <v>147</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1891,7 +1890,7 @@
         <v>148</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1905,7 +1904,7 @@
         <v>149</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1919,7 +1918,7 @@
         <v>150</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1933,7 +1932,7 @@
         <v>151</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -1942,16 +1941,16 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF3F758D-F5D4-974E-8C16-A079BD7221FD}">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E0222B4-433A-4847-9EF9-ED7322586C33}">
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>13</v>
       </c>
@@ -1965,70 +1964,59 @@
         <v>2</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="C2" s="3">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="E2" t="s">
-        <v>155</v>
-      </c>
-      <c r="F2" s="3">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="C2" s="7">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="E2" s="7">
+        <v>0.03</v>
+      </c>
+      <c r="F2" s="7">
+        <v>0.03</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="E3" t="s">
-        <v>157</v>
-      </c>
-      <c r="F3" s="3">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="7">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="E4" t="s">
-        <v>159</v>
-      </c>
-      <c r="F4" s="3">
-        <v>1000</v>
+      <c r="B3" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="C3" s="7">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0.03</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0.03</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -2037,81 +2025,6 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E0222B4-433A-4847-9EF9-ED7322586C33}">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18:E19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="9">
-        <v>0</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="C2" s="9">
-        <v>1</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="E2" s="9">
-        <v>0.03</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="9">
-        <v>1</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="C3" s="9">
-        <v>1</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="E3" s="9">
-        <v>0.03</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{369B7ED6-0339-A34F-8D4C-28B9C408DB19}">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -2132,10 +2045,10 @@
         <v>51</v>
       </c>
       <c r="D1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="E1" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -2143,7 +2056,7 @@
         <v>79</v>
       </c>
       <c r="B2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C2" t="s">
         <v>70</v>
@@ -2160,7 +2073,7 @@
         <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C3" t="s">
         <v>71</v>
@@ -2177,7 +2090,7 @@
         <v>83</v>
       </c>
       <c r="B4" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C4" t="s">
         <v>76</v>
@@ -2194,7 +2107,7 @@
         <v>85</v>
       </c>
       <c r="B5" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C5" t="s">
         <v>77</v>
@@ -2211,7 +2124,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23BC4103-A416-3E41-9041-99544891E416}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2222,62 +2135,62 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="9" t="s">
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="F1" s="9" t="s">
+      <c r="E1" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="9">
-        <v>0</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="C2" s="9">
-        <v>1</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="E2" s="9">
+      <c r="A2" s="7">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="7">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="E2" s="7">
         <v>0.03</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="7" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="9">
-        <v>1</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="C3" s="9">
-        <v>1</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="E3" s="9">
+      <c r="A3" s="7">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C3" s="7">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="E3" s="7">
         <v>0.03</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="7" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2286,7 +2199,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB172BE7-B3C0-A449-8F62-0781AC3DED02}">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -2307,7 +2220,7 @@
         <v>51</v>
       </c>
       <c r="D1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2315,7 +2228,7 @@
         <v>79</v>
       </c>
       <c r="B2" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C2" t="s">
         <v>70</v>
@@ -2329,7 +2242,7 @@
         <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C3" t="s">
         <v>71</v>
@@ -2343,7 +2256,7 @@
         <v>83</v>
       </c>
       <c r="B4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C4" t="s">
         <v>76</v>
@@ -2357,13 +2270,88 @@
         <v>85</v>
       </c>
       <c r="B5" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C5" t="s">
         <v>77</v>
       </c>
       <c r="D5" s="3">
         <v>0.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{145CFC81-A232-1D4D-AC9D-AC7308213471}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="7">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="C2" s="7">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E2" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="7">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C3" s="7">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -2372,81 +2360,6 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{145CFC81-A232-1D4D-AC9D-AC7308213471}">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L39" sqref="L39"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="9">
-        <v>0</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="C2" s="9">
-        <v>1</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="E2" s="9">
-        <v>0.05</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="9">
-        <v>1</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="C3" s="9">
-        <v>1</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="E3" s="9">
-        <v>0.05</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF8DCDA-3E95-6745-801C-7005462F6D2D}">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -2467,7 +2380,7 @@
         <v>51</v>
       </c>
       <c r="D1" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2475,7 +2388,7 @@
         <v>79</v>
       </c>
       <c r="B2" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C2" t="s">
         <v>70</v>
@@ -2489,7 +2402,7 @@
         <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C3" t="s">
         <v>71</v>
@@ -2503,7 +2416,7 @@
         <v>83</v>
       </c>
       <c r="B4" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C4" t="s">
         <v>76</v>
@@ -2517,7 +2430,7 @@
         <v>85</v>
       </c>
       <c r="B5" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C5" t="s">
         <v>77</v>
@@ -2847,7 +2760,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2879,7 +2792,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -2911,7 +2824,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -2950,7 +2863,7 @@
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R2" sqref="R2:S2"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3008,10 +2921,10 @@
         <v>5</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>26</v>
@@ -3019,8 +2932,8 @@
       <c r="U1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
@@ -3045,7 +2958,7 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>2.1</v>
+        <v>1</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -3217,7 +3130,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:V9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
     </sheetView>
@@ -3276,11 +3189,11 @@
       <c r="Q1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="R1" s="12" t="s">
-        <v>214</v>
-      </c>
-      <c r="S1" s="12" t="s">
-        <v>215</v>
+      <c r="R1" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="S1" s="10" t="s">
+        <v>210</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>26</v>
@@ -3358,8 +3271,8 @@
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="R9" s="13"/>
-      <c r="S9" s="13"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3367,17 +3280,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:X8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0A0BCC1-5090-3645-97C9-41B78CF5D933}">
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -3391,518 +3303,164 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>0</v>
+      <c r="B2" t="s">
+        <v>62</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
+        <v>62</v>
+      </c>
+      <c r="E2" t="s">
+        <v>70</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>230</v>
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>230</v>
+        <v>1450</v>
       </c>
       <c r="K2">
-        <v>2.81E-3</v>
-      </c>
-      <c r="L2">
-        <v>2.81E-2</v>
-      </c>
-      <c r="M2">
-        <v>7.1199999999999996E-3</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2">
-        <v>1</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>1</v>
+      <c r="B3" t="s">
+        <v>63</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
+        <v>63</v>
+      </c>
+      <c r="E3" t="s">
+        <v>71</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G3">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>230</v>
+        <v>0</v>
       </c>
       <c r="J3">
-        <v>230</v>
+        <v>3000</v>
       </c>
       <c r="K3">
-        <v>3.0400000000000002E-3</v>
-      </c>
-      <c r="L3">
-        <v>3.04E-2</v>
-      </c>
-      <c r="M3">
-        <v>6.5799999999999999E-3</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3">
-        <v>1</v>
-      </c>
-      <c r="U3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4">
         <v>2</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>4</v>
-      </c>
       <c r="G4">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>230</v>
+        <v>0</v>
       </c>
       <c r="J4">
-        <v>230</v>
+        <v>4000</v>
       </c>
       <c r="K4">
-        <v>6.4000000000000005E-4</v>
-      </c>
-      <c r="L4">
-        <v>6.4000000000000003E-3</v>
-      </c>
-      <c r="M4">
-        <v>3.1260000000000003E-2</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4">
-        <v>1</v>
-      </c>
-      <c r="U4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>3</v>
+      <c r="B5" t="s">
+        <v>65</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
+        <v>65</v>
+      </c>
+      <c r="E5" t="s">
+        <v>77</v>
       </c>
       <c r="F5">
         <v>2</v>
       </c>
       <c r="G5">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>230</v>
+        <v>0</v>
       </c>
       <c r="J5">
-        <v>230</v>
+        <v>3000</v>
       </c>
       <c r="K5">
-        <v>1.08E-3</v>
-      </c>
-      <c r="L5">
-        <v>1.0800000000000001E-2</v>
-      </c>
-      <c r="M5">
-        <v>1.8519999999999998E-2</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5">
-        <v>1</v>
-      </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>4</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6">
-        <v>3</v>
-      </c>
-      <c r="G6">
-        <v>100</v>
-      </c>
-      <c r="H6">
-        <v>60</v>
-      </c>
-      <c r="I6">
-        <v>230</v>
-      </c>
-      <c r="J6">
-        <v>230</v>
-      </c>
-      <c r="K6">
-        <v>2.97E-3</v>
-      </c>
-      <c r="L6">
-        <v>2.9700000000000001E-2</v>
-      </c>
-      <c r="M6">
-        <v>6.7400000000000003E-3</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="R6">
-        <v>0</v>
-      </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-      <c r="T6">
-        <v>1</v>
-      </c>
-      <c r="U6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>5</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7">
-        <v>3</v>
-      </c>
-      <c r="F7">
-        <v>4</v>
-      </c>
-      <c r="G7">
-        <v>100</v>
-      </c>
-      <c r="H7">
-        <v>60</v>
-      </c>
-      <c r="I7">
-        <v>230</v>
-      </c>
-      <c r="J7">
-        <v>230</v>
-      </c>
-      <c r="K7">
-        <v>2.97E-3</v>
-      </c>
-      <c r="L7">
-        <v>2.9700000000000001E-2</v>
-      </c>
-      <c r="M7">
-        <v>6.7400000000000003E-3</v>
-      </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="R7">
-        <v>0</v>
-      </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-      <c r="T7">
-        <v>1</v>
-      </c>
-      <c r="U7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>6</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>100</v>
-      </c>
-      <c r="H8">
-        <v>60</v>
-      </c>
-      <c r="I8">
-        <v>230</v>
-      </c>
-      <c r="J8">
-        <v>230</v>
-      </c>
-      <c r="K8">
-        <v>2.81E-3</v>
-      </c>
-      <c r="L8">
-        <v>2.81E-2</v>
-      </c>
-      <c r="M8">
-        <v>7.1199999999999996E-3</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-      <c r="T8">
-        <v>1</v>
-      </c>
-      <c r="U8">
         <v>0</v>
       </c>
     </row>
@@ -3912,6 +3470,623 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:AA8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O11" sqref="O11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>100</v>
+      </c>
+      <c r="H2">
+        <v>60</v>
+      </c>
+      <c r="I2">
+        <v>230</v>
+      </c>
+      <c r="J2">
+        <v>230</v>
+      </c>
+      <c r="K2">
+        <v>2.81E-3</v>
+      </c>
+      <c r="L2">
+        <v>2.81E-2</v>
+      </c>
+      <c r="M2">
+        <v>7.1199999999999996E-3</v>
+      </c>
+      <c r="N2">
+        <v>999</v>
+      </c>
+      <c r="O2">
+        <v>999</v>
+      </c>
+      <c r="P2">
+        <v>999</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>1</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>100</v>
+      </c>
+      <c r="H3">
+        <v>60</v>
+      </c>
+      <c r="I3">
+        <v>230</v>
+      </c>
+      <c r="J3">
+        <v>230</v>
+      </c>
+      <c r="K3">
+        <v>3.0400000000000002E-3</v>
+      </c>
+      <c r="L3">
+        <v>3.04E-2</v>
+      </c>
+      <c r="M3">
+        <v>6.5799999999999999E-3</v>
+      </c>
+      <c r="N3">
+        <v>999</v>
+      </c>
+      <c r="O3">
+        <v>999</v>
+      </c>
+      <c r="P3">
+        <v>999</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>1</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>100</v>
+      </c>
+      <c r="H4">
+        <v>60</v>
+      </c>
+      <c r="I4">
+        <v>230</v>
+      </c>
+      <c r="J4">
+        <v>230</v>
+      </c>
+      <c r="K4">
+        <v>6.4000000000000005E-4</v>
+      </c>
+      <c r="L4">
+        <v>6.4000000000000003E-3</v>
+      </c>
+      <c r="M4">
+        <v>3.1260000000000003E-2</v>
+      </c>
+      <c r="N4">
+        <v>999</v>
+      </c>
+      <c r="O4">
+        <v>999</v>
+      </c>
+      <c r="P4">
+        <v>999</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>1</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>100</v>
+      </c>
+      <c r="H5">
+        <v>60</v>
+      </c>
+      <c r="I5">
+        <v>230</v>
+      </c>
+      <c r="J5">
+        <v>230</v>
+      </c>
+      <c r="K5">
+        <v>1.08E-3</v>
+      </c>
+      <c r="L5">
+        <v>1.0800000000000001E-2</v>
+      </c>
+      <c r="M5">
+        <v>1.8519999999999998E-2</v>
+      </c>
+      <c r="N5">
+        <v>999</v>
+      </c>
+      <c r="O5">
+        <v>999</v>
+      </c>
+      <c r="P5">
+        <v>999</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>1</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>100</v>
+      </c>
+      <c r="H6">
+        <v>60</v>
+      </c>
+      <c r="I6">
+        <v>230</v>
+      </c>
+      <c r="J6">
+        <v>230</v>
+      </c>
+      <c r="K6">
+        <v>2.97E-3</v>
+      </c>
+      <c r="L6">
+        <v>2.9700000000000001E-2</v>
+      </c>
+      <c r="M6">
+        <v>6.7400000000000003E-3</v>
+      </c>
+      <c r="N6">
+        <v>999</v>
+      </c>
+      <c r="O6">
+        <v>999</v>
+      </c>
+      <c r="P6">
+        <v>999</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>1</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>100</v>
+      </c>
+      <c r="H7">
+        <v>60</v>
+      </c>
+      <c r="I7">
+        <v>230</v>
+      </c>
+      <c r="J7">
+        <v>230</v>
+      </c>
+      <c r="K7">
+        <v>2.97E-3</v>
+      </c>
+      <c r="L7">
+        <v>2.9700000000000001E-2</v>
+      </c>
+      <c r="M7">
+        <v>6.7400000000000003E-3</v>
+      </c>
+      <c r="N7">
+        <v>999</v>
+      </c>
+      <c r="O7">
+        <v>999</v>
+      </c>
+      <c r="P7">
+        <v>999</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>1</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>100</v>
+      </c>
+      <c r="H8">
+        <v>60</v>
+      </c>
+      <c r="I8">
+        <v>230</v>
+      </c>
+      <c r="J8">
+        <v>230</v>
+      </c>
+      <c r="K8">
+        <v>2.81E-3</v>
+      </c>
+      <c r="L8">
+        <v>2.81E-2</v>
+      </c>
+      <c r="M8">
+        <v>7.1199999999999996E-3</v>
+      </c>
+      <c r="N8">
+        <v>999</v>
+      </c>
+      <c r="O8">
+        <v>999</v>
+      </c>
+      <c r="P8">
+        <v>999</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>1</v>
+      </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -3974,7 +4149,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AB94B98-B38A-EC46-833E-965628D04701}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -4017,203 +4192,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C3" s="4">
         <v>1</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>55</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0A0BCC1-5090-3645-97C9-41B78CF5D933}">
-  <dimension ref="A1:K5"/>
-  <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>1450</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>3000</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>1000</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>65</v>
-      </c>
-      <c r="E5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>3000</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[WIP] Clean up cases
</commit_message>
<xml_diff>
--- a/ams/cases/5bus/pjm5bus_uced.xlsx
+++ b/ams/cases/5bus/pjm5bus_uced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/ams/ams/cases/5bus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{844ECDA7-4567-8542-97E2-144FADC54E13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C355EB6-8FD3-714D-87C9-34D33F2A161E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21600" yWindow="2660" windowWidth="21600" windowHeight="18940" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2380" yWindow="2000" windowWidth="22780" windowHeight="15700" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="21" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="220">
   <si>
     <t>idx</t>
   </si>
@@ -703,6 +703,12 @@
   </si>
   <si>
     <t>rate_c</t>
+  </si>
+  <si>
+    <t>ug</t>
+  </si>
+  <si>
+    <t>1,1,1,1</t>
   </si>
 </sst>
 </file>
@@ -1212,15 +1218,15 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{787DEB6E-5407-D64E-8FD6-1F71A62EBC04}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -1233,8 +1239,11 @@
       <c r="D1" s="5" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>79</v>
       </c>
@@ -1247,8 +1256,11 @@
       <c r="D2" s="6" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -1261,8 +1273,11 @@
       <c r="D3" s="6" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>83</v>
       </c>
@@ -1275,8 +1290,11 @@
       <c r="D4" s="6" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>85</v>
       </c>
@@ -1289,8 +1307,11 @@
       <c r="D5" s="6" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>87</v>
       </c>
@@ -1303,8 +1324,11 @@
       <c r="D6" s="6" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>89</v>
       </c>
@@ -1317,8 +1341,11 @@
       <c r="D7" s="6" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E7" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>91</v>
       </c>
@@ -1331,8 +1358,11 @@
       <c r="D8" s="6" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>93</v>
       </c>
@@ -1345,8 +1375,11 @@
       <c r="D9" s="6" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>95</v>
       </c>
@@ -1359,8 +1392,11 @@
       <c r="D10" s="6" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E10" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>97</v>
       </c>
@@ -1373,8 +1409,11 @@
       <c r="D11" s="6" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>99</v>
       </c>
@@ -1387,8 +1426,11 @@
       <c r="D12" s="6" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E12" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>101</v>
       </c>
@@ -1401,8 +1443,11 @@
       <c r="D13" s="6" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E13" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>103</v>
       </c>
@@ -1415,8 +1460,11 @@
       <c r="D14" s="6" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E14" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>105</v>
       </c>
@@ -1429,8 +1477,11 @@
       <c r="D15" s="6" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E15" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>107</v>
       </c>
@@ -1443,8 +1494,11 @@
       <c r="D16" s="6" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E16" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>109</v>
       </c>
@@ -1457,8 +1511,11 @@
       <c r="D17" s="6" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E17" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>111</v>
       </c>
@@ -1471,8 +1528,11 @@
       <c r="D18" s="6" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>113</v>
       </c>
@@ -1485,8 +1545,11 @@
       <c r="D19" s="6" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>115</v>
       </c>
@@ -1499,8 +1562,11 @@
       <c r="D20" s="6" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E20" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>118</v>
       </c>
@@ -1513,8 +1579,11 @@
       <c r="D21" s="6" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E21" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>120</v>
       </c>
@@ -1527,8 +1596,11 @@
       <c r="D22" s="6" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E22" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>122</v>
       </c>
@@ -1541,8 +1613,11 @@
       <c r="D23" s="6" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E23" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>124</v>
       </c>
@@ -1555,8 +1630,11 @@
       <c r="D24" s="6" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E24" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>126</v>
       </c>
@@ -1569,8 +1647,12 @@
       <c r="D25" s="6" t="s">
         <v>198</v>
       </c>
+      <c r="E25" t="s">
+        <v>219</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3283,7 +3365,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0A0BCC1-5090-3645-97C9-41B78CF5D933}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix PJM case cost and line rate
</commit_message>
<xml_diff>
--- a/ams/cases/5bus/pjm5bus_uced.xlsx
+++ b/ams/cases/5bus/pjm5bus_uced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/ams/ams/cases/5bus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C355EB6-8FD3-714D-87C9-34D33F2A161E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AEA5562-9E18-F44E-9FE2-810173E7FA9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2380" yWindow="2000" windowWidth="22780" windowHeight="15700" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1540" windowWidth="34560" windowHeight="19000" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="21" r:id="rId1"/>
@@ -183,27 +183,6 @@
     <t>phi</t>
   </si>
   <si>
-    <t>Line 1-2</t>
-  </si>
-  <si>
-    <t>Line 1-4</t>
-  </si>
-  <si>
-    <t>Line 1-5</t>
-  </si>
-  <si>
-    <t>Line 2-3</t>
-  </si>
-  <si>
-    <t>Line 3-4</t>
-  </si>
-  <si>
-    <t>Line 4-5</t>
-  </si>
-  <si>
-    <t>Line 1-2 (2)</t>
-  </si>
-  <si>
     <t>gen</t>
   </si>
   <si>
@@ -709,6 +688,27 @@
   </si>
   <si>
     <t>1,1,1,1</t>
+  </si>
+  <si>
+    <t>Line AB</t>
+  </si>
+  <si>
+    <t>Line AD</t>
+  </si>
+  <si>
+    <t>Line AE</t>
+  </si>
+  <si>
+    <t>Line BC</t>
+  </si>
+  <si>
+    <t>Line CD</t>
+  </si>
+  <si>
+    <t>Line DE</t>
+  </si>
+  <si>
+    <t>Line AB2</t>
   </si>
 </sst>
 </file>
@@ -1164,16 +1164,16 @@
         <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1181,10 +1181,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
@@ -1194,10 +1194,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C3" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1205,10 +1205,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="C4" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -1220,7 +1220,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{787DEB6E-5407-D64E-8FD6-1F71A62EBC04}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
@@ -1237,418 +1237,418 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E1" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="E2" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="E3" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="E4" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="E5" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="E6" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="E7" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="E8" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="E9" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="E10" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="E11" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="E12" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="E13" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="E14" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="E15" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="E16" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="E17" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="E18" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="E19" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="E20" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="E21" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="E22" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="E23" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="E24" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="E25" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -1678,343 +1678,343 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -2046,10 +2046,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>11</v>
@@ -2060,13 +2060,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="C2" s="7">
         <v>1</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="E2" s="7">
         <v>0.03</v>
@@ -2075,7 +2075,7 @@
         <v>0.03</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -2083,13 +2083,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="C3" s="7">
         <v>1</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="E3" s="7">
         <v>0.03</v>
@@ -2098,7 +2098,7 @@
         <v>0.03</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -2124,81 +2124,81 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D1" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="E1" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D3" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E3" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B4" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C4" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D4" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E4" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B5" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D5" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E5" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -2230,7 +2230,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>11</v>
@@ -2241,19 +2241,19 @@
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C2" s="7">
         <v>1</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="E2" s="7">
         <v>0.03</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -2261,19 +2261,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="C3" s="7">
         <v>1</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="E3" s="7">
         <v>0.03</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -2299,21 +2299,21 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D1" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D2" s="3">
         <v>0.1</v>
@@ -2321,13 +2321,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D3" s="3">
         <v>0.1</v>
@@ -2335,13 +2335,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B4" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="C4" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D4" s="3">
         <v>0.1</v>
@@ -2349,13 +2349,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B5" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D5" s="3">
         <v>0.1</v>
@@ -2390,7 +2390,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>11</v>
@@ -2401,19 +2401,19 @@
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="C2" s="7">
         <v>1</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="E2" s="7">
         <v>0.01</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -2421,19 +2421,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C3" s="7">
         <v>1</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="E3" s="7">
         <v>0.01</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -2459,21 +2459,21 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D2" s="3">
         <v>0.1</v>
@@ -2481,13 +2481,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D3" s="3">
         <v>0.1</v>
@@ -2495,13 +2495,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B4" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="C4" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D4" s="3">
         <v>0.1</v>
@@ -2509,13 +2509,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B5" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D5" s="3">
         <v>0.1</v>
@@ -2532,7 +2532,7 @@
   <sheetViews>
     <sheetView zoomScale="118" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M10" sqref="M10"/>
+      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2592,7 +2592,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="E2">
         <v>230</v>
@@ -2619,7 +2619,7 @@
         <v>1</v>
       </c>
       <c r="M2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -2633,7 +2633,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="E3">
         <v>230</v>
@@ -2660,7 +2660,7 @@
         <v>1</v>
       </c>
       <c r="M3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -2674,7 +2674,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="E4">
         <v>230</v>
@@ -2701,7 +2701,7 @@
         <v>2</v>
       </c>
       <c r="M4" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -2715,7 +2715,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="E5">
         <v>230</v>
@@ -2742,7 +2742,7 @@
         <v>2</v>
       </c>
       <c r="M5" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -2756,7 +2756,7 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E6">
         <v>230</v>
@@ -2783,7 +2783,7 @@
         <v>3</v>
       </c>
       <c r="M6" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -2842,7 +2842,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2874,7 +2874,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -2906,7 +2906,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -3003,10 +3003,10 @@
         <v>5</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>26</v>
@@ -3022,13 +3022,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E2">
         <v>100</v>
@@ -3084,13 +3084,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E3">
         <v>100</v>
@@ -3146,13 +3146,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="E4">
         <v>100</v>
@@ -3272,10 +3272,10 @@
         <v>5</v>
       </c>
       <c r="R1" s="10" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="S1" s="10" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>26</v>
@@ -3292,13 +3292,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E2">
         <v>100</v>
@@ -3366,7 +3366,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3385,25 +3385,25 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -3411,16 +3411,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="F2">
         <v>2</v>
@@ -3435,7 +3435,7 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>1450</v>
+        <v>0.14499999999999999</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -3446,16 +3446,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -3470,7 +3470,7 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>3000</v>
+        <v>0.3</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -3481,16 +3481,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E4" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -3505,7 +3505,7 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>4000</v>
+        <v>0.4</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -3516,16 +3516,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E5" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F5">
         <v>2</v>
@@ -3540,7 +3540,7 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>3000</v>
+        <v>0.1</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -3555,9 +3555,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="165" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O11" sqref="O11"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3603,13 +3603,13 @@
         <v>35</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>36</v>
@@ -3656,7 +3656,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>213</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -3686,13 +3686,13 @@
         <v>7.1199999999999996E-3</v>
       </c>
       <c r="N2">
-        <v>999</v>
+        <v>4</v>
       </c>
       <c r="O2">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -3730,7 +3730,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>214</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -3760,13 +3760,13 @@
         <v>6.5799999999999999E-3</v>
       </c>
       <c r="N3">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="O3">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -3804,7 +3804,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>215</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -3834,13 +3834,13 @@
         <v>3.1260000000000003E-2</v>
       </c>
       <c r="N4">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="O4">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="P4">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="Q4">
         <v>0</v>
@@ -3878,7 +3878,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>216</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -3908,13 +3908,13 @@
         <v>1.8519999999999998E-2</v>
       </c>
       <c r="N5">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="O5">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="P5">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="Q5">
         <v>0</v>
@@ -3952,7 +3952,7 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>217</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -3982,13 +3982,13 @@
         <v>6.7400000000000003E-3</v>
       </c>
       <c r="N6">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="O6">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="P6">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="Q6">
         <v>0</v>
@@ -4026,7 +4026,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>218</v>
       </c>
       <c r="E7">
         <v>3</v>
@@ -4056,13 +4056,13 @@
         <v>6.7400000000000003E-3</v>
       </c>
       <c r="N7">
-        <v>999</v>
+        <v>2.4</v>
       </c>
       <c r="O7">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="P7">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="Q7">
         <v>0</v>
@@ -4100,7 +4100,7 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>50</v>
+        <v>219</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -4130,13 +4130,13 @@
         <v>7.1199999999999996E-3</v>
       </c>
       <c r="N8">
-        <v>999</v>
+        <v>4</v>
       </c>
       <c r="O8">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="P8">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="Q8">
         <v>0</v>
@@ -4260,13 +4260,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C2" s="4">
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4274,13 +4274,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="C3" s="4">
         <v>1</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add case pjm5bus_demo for demo purpose with reduced timeslot data
</commit_message>
<xml_diff>
--- a/ams/cases/5bus/pjm5bus_uced.xlsx
+++ b/ams/cases/5bus/pjm5bus_uced.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/ams/ams/cases/5bus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5809E77A-CAC1-9C49-B99E-A7F93FAB9AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD8E34D-2189-4C4C-8C5A-F7959CEACDC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1540" windowWidth="34560" windowHeight="19000" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1540" windowWidth="34560" windowHeight="19000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="21" r:id="rId1"/>
@@ -18,19 +18,19 @@
     <sheet name="PQ" sheetId="2" r:id="rId3"/>
     <sheet name="PV" sheetId="3" r:id="rId4"/>
     <sheet name="Slack" sheetId="4" r:id="rId5"/>
-    <sheet name="GCost" sheetId="11" r:id="rId6"/>
-    <sheet name="Line" sheetId="5" r:id="rId7"/>
-    <sheet name="Area" sheetId="6" r:id="rId8"/>
-    <sheet name="Region" sheetId="10" r:id="rId9"/>
-    <sheet name="EDTSlot" sheetId="12" r:id="rId10"/>
-    <sheet name="UCTSlot" sheetId="13" r:id="rId11"/>
-    <sheet name="SFR" sheetId="15" r:id="rId12"/>
-    <sheet name="SFRCost" sheetId="16" r:id="rId13"/>
-    <sheet name="SR" sheetId="17" r:id="rId14"/>
-    <sheet name="SRCost" sheetId="18" r:id="rId15"/>
-    <sheet name="NSR" sheetId="19" r:id="rId16"/>
-    <sheet name="NSRCost" sheetId="20" r:id="rId17"/>
-    <sheet name="DCost" sheetId="22" r:id="rId18"/>
+    <sheet name="Line" sheetId="5" r:id="rId6"/>
+    <sheet name="Area" sheetId="6" r:id="rId7"/>
+    <sheet name="Region" sheetId="10" r:id="rId8"/>
+    <sheet name="GCost" sheetId="11" r:id="rId9"/>
+    <sheet name="SRCost" sheetId="18" r:id="rId10"/>
+    <sheet name="SFRCost" sheetId="16" r:id="rId11"/>
+    <sheet name="DCost" sheetId="22" r:id="rId12"/>
+    <sheet name="NSRCost" sheetId="20" r:id="rId13"/>
+    <sheet name="EDTSlot" sheetId="12" r:id="rId14"/>
+    <sheet name="UCTSlot" sheetId="13" r:id="rId15"/>
+    <sheet name="SFR" sheetId="15" r:id="rId16"/>
+    <sheet name="SR" sheetId="17" r:id="rId17"/>
+    <sheet name="NSR" sheetId="19" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="247">
   <si>
     <t>idx</t>
   </si>
@@ -737,6 +737,60 @@
   </si>
   <si>
     <t>Dcost 3</t>
+  </si>
+  <si>
+    <t>Line_0</t>
+  </si>
+  <si>
+    <t>Line_1</t>
+  </si>
+  <si>
+    <t>Line_2</t>
+  </si>
+  <si>
+    <t>Line_3</t>
+  </si>
+  <si>
+    <t>Line_4</t>
+  </si>
+  <si>
+    <t>Line_5</t>
+  </si>
+  <si>
+    <t>Line_6</t>
+  </si>
+  <si>
+    <t>Bus_1</t>
+  </si>
+  <si>
+    <t>Bus_2</t>
+  </si>
+  <si>
+    <t>Bus_3</t>
+  </si>
+  <si>
+    <t>Bus_4</t>
+  </si>
+  <si>
+    <t>Bus_5</t>
+  </si>
+  <si>
+    <t>ZONE 1</t>
+  </si>
+  <si>
+    <t>ZONE 2</t>
+  </si>
+  <si>
+    <t>Gcost 1</t>
+  </si>
+  <si>
+    <t>Gcost 2</t>
+  </si>
+  <si>
+    <t>Gcost 3</t>
+  </si>
+  <si>
+    <t>Gcost 4</t>
   </si>
 </sst>
 </file>
@@ -1288,6 +1342,371 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB172BE7-B3C0-A449-8F62-0781AC3DED02}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{369B7ED6-0339-A34F-8D4C-28B9C408DB19}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{130608C9-3E81-B940-B421-2E5FE1C369EA}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView zoomScale="108" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="14">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="14">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E3" t="s">
+        <v>146</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="14">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E4" t="s">
+        <v>147</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF8DCDA-3E95-6745-801C-7005462F6D2D}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J43" sqref="J43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" t="s">
+        <v>168</v>
+      </c>
+      <c r="C5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{787DEB6E-5407-D64E-8FD6-1F71A62EBC04}">
   <dimension ref="A1:E25"/>
   <sheetViews>
@@ -1728,7 +2147,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2777B7D7-CE5C-114E-9B38-A548A06A92E7}">
   <dimension ref="A1:D25"/>
   <sheetViews>
@@ -2093,7 +2512,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E0222B4-433A-4847-9EF9-ED7322586C33}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -2177,107 +2596,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{369B7ED6-0339-A34F-8D4C-28B9C408DB19}">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" t="s">
-        <v>158</v>
-      </c>
-      <c r="C2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" t="s">
-        <v>159</v>
-      </c>
-      <c r="C3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" t="s">
-        <v>160</v>
-      </c>
-      <c r="C4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B5" t="s">
-        <v>161</v>
-      </c>
-      <c r="C5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23BC4103-A416-3E41-9041-99544891E416}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2352,92 +2671,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB172BE7-B3C0-A449-8F62-0781AC3DED02}">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" t="s">
-        <v>152</v>
-      </c>
-      <c r="C2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" t="s">
-        <v>153</v>
-      </c>
-      <c r="C3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" t="s">
-        <v>154</v>
-      </c>
-      <c r="C4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B5" t="s">
-        <v>155</v>
-      </c>
-      <c r="C5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0.1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{145CFC81-A232-1D4D-AC9D-AC7308213471}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2512,193 +2746,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF8DCDA-3E95-6745-801C-7005462F6D2D}">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L41" sqref="L41"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" t="s">
-        <v>165</v>
-      </c>
-      <c r="C2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" t="s">
-        <v>166</v>
-      </c>
-      <c r="C3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" t="s">
-        <v>167</v>
-      </c>
-      <c r="C4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B5" t="s">
-        <v>168</v>
-      </c>
-      <c r="C5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0.1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{130608C9-3E81-B940-B421-2E5FE1C369EA}">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>221</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="14">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="C2" s="2">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="E2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F2" s="2">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="14">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="E3" t="s">
-        <v>146</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="14">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="E4" t="s">
-        <v>147</v>
-      </c>
-      <c r="F4" s="2">
-        <v>1000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView zoomScale="118" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="118" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2751,8 +2805,8 @@
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>0</v>
+      <c r="B2" t="s">
+        <v>236</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2792,8 +2846,8 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>1</v>
+      <c r="B3" t="s">
+        <v>237</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -2833,8 +2887,8 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>2</v>
+      <c r="B4" t="s">
+        <v>238</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -2874,8 +2928,8 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>3</v>
+      <c r="B5" t="s">
+        <v>239</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -2915,8 +2969,8 @@
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>4</v>
+      <c r="B6" t="s">
+        <v>240</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -2953,6 +3007,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2963,7 +3018,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q23" sqref="Q23"/>
+      <selection pane="bottomLeft" activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3019,8 +3074,8 @@
       <c r="D2" t="s">
         <v>17</v>
       </c>
-      <c r="E2">
-        <v>1</v>
+      <c r="E2" t="s">
+        <v>237</v>
       </c>
       <c r="F2">
         <v>230</v>
@@ -3054,8 +3109,8 @@
       <c r="D3" t="s">
         <v>18</v>
       </c>
-      <c r="E3">
-        <v>2</v>
+      <c r="E3" t="s">
+        <v>238</v>
       </c>
       <c r="F3">
         <v>230</v>
@@ -3089,8 +3144,8 @@
       <c r="D4" t="s">
         <v>19</v>
       </c>
-      <c r="E4">
-        <v>3</v>
+      <c r="E4" t="s">
+        <v>239</v>
       </c>
       <c r="F4">
         <v>230</v>
@@ -3123,7 +3178,7 @@
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3214,8 +3269,8 @@
       <c r="F2">
         <v>230</v>
       </c>
-      <c r="G2">
-        <v>0</v>
+      <c r="G2" t="s">
+        <v>236</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -3276,8 +3331,8 @@
       <c r="F3">
         <v>230</v>
       </c>
-      <c r="G3">
-        <v>2</v>
+      <c r="G3" t="s">
+        <v>238</v>
       </c>
       <c r="I3">
         <v>3.2349000000000001</v>
@@ -3338,8 +3393,8 @@
       <c r="F4">
         <v>230</v>
       </c>
-      <c r="G4">
-        <v>4</v>
+      <c r="G4" t="s">
+        <v>240</v>
       </c>
       <c r="I4">
         <v>4.6650999999999998</v>
@@ -3392,7 +3447,7 @@
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3484,8 +3539,8 @@
       <c r="F2">
         <v>230</v>
       </c>
-      <c r="G2">
-        <v>3</v>
+      <c r="G2" t="s">
+        <v>239</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -3540,202 +3595,12 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0A0BCC1-5090-3645-97C9-41B78CF5D933}">
-  <dimension ref="A1:K5"/>
-  <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0.14499999999999999</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0.3</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0.4</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0.1</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
     <sheetView zoomScale="165" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3827,8 +3692,8 @@
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>0</v>
+      <c r="B2" t="s">
+        <v>229</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -3836,11 +3701,11 @@
       <c r="D2" t="s">
         <v>213</v>
       </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
+      <c r="E2" t="s">
+        <v>236</v>
+      </c>
+      <c r="F2" t="s">
+        <v>237</v>
       </c>
       <c r="G2">
         <v>100</v>
@@ -3901,8 +3766,8 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>1</v>
+      <c r="B3" t="s">
+        <v>230</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -3910,11 +3775,11 @@
       <c r="D3" t="s">
         <v>214</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>3</v>
+      <c r="E3" t="s">
+        <v>236</v>
+      </c>
+      <c r="F3" t="s">
+        <v>239</v>
       </c>
       <c r="G3">
         <v>100</v>
@@ -3975,8 +3840,8 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>2</v>
+      <c r="B4" t="s">
+        <v>231</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -3984,11 +3849,11 @@
       <c r="D4" t="s">
         <v>215</v>
       </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>4</v>
+      <c r="E4" t="s">
+        <v>236</v>
+      </c>
+      <c r="F4" t="s">
+        <v>240</v>
       </c>
       <c r="G4">
         <v>100</v>
@@ -4049,8 +3914,8 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>3</v>
+      <c r="B5" t="s">
+        <v>232</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -4058,11 +3923,11 @@
       <c r="D5" t="s">
         <v>216</v>
       </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
+      <c r="E5" t="s">
+        <v>237</v>
+      </c>
+      <c r="F5" t="s">
+        <v>238</v>
       </c>
       <c r="G5">
         <v>100</v>
@@ -4123,8 +3988,8 @@
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>4</v>
+      <c r="B6" t="s">
+        <v>233</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -4132,11 +3997,11 @@
       <c r="D6" t="s">
         <v>217</v>
       </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6">
-        <v>3</v>
+      <c r="E6" t="s">
+        <v>238</v>
+      </c>
+      <c r="F6" t="s">
+        <v>239</v>
       </c>
       <c r="G6">
         <v>100</v>
@@ -4197,8 +4062,8 @@
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7">
-        <v>5</v>
+      <c r="B7" t="s">
+        <v>234</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -4206,11 +4071,11 @@
       <c r="D7" t="s">
         <v>218</v>
       </c>
-      <c r="E7">
-        <v>3</v>
-      </c>
-      <c r="F7">
-        <v>4</v>
+      <c r="E7" t="s">
+        <v>239</v>
+      </c>
+      <c r="F7" t="s">
+        <v>240</v>
       </c>
       <c r="G7">
         <v>100</v>
@@ -4271,8 +4136,8 @@
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8">
-        <v>6</v>
+      <c r="B8" t="s">
+        <v>235</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -4280,11 +4145,11 @@
       <c r="D8" t="s">
         <v>219</v>
       </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
+      <c r="E8" t="s">
+        <v>236</v>
+      </c>
+      <c r="F8" t="s">
+        <v>237</v>
       </c>
       <c r="G8">
         <v>100</v>
@@ -4342,11 +4207,12 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -4409,12 +4275,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AB94B98-B38A-EC46-833E-965628D04701}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4444,7 +4310,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>47</v>
+        <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4458,10 +4324,201 @@
         <v>1</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>48</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0A0BCC1-5090-3645-97C9-41B78CF5D933}">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>243</v>
+      </c>
+      <c r="E2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0.3</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>245</v>
+      </c>
+      <c r="E4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0.4</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>246</v>
+      </c>
+      <c r="E5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0.1</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>